<commit_message>
All data for CAs up to present day. Some missing data represented with ?
</commit_message>
<xml_diff>
--- a/CAFamilyData.xlsx
+++ b/CAFamilyData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="760" windowWidth="18640" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="2240" yWindow="2320" windowWidth="26560" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="282">
   <si>
     <t>Name</t>
   </si>
@@ -595,13 +595,283 @@
   </si>
   <si>
     <t>Section</t>
+  </si>
+  <si>
+    <t>Alex Smith</t>
+  </si>
+  <si>
+    <t>amsmith1</t>
+  </si>
+  <si>
+    <t>cwswanso</t>
+  </si>
+  <si>
+    <t>Charlie Swanson</t>
+  </si>
+  <si>
+    <t>Tom Abraham</t>
+  </si>
+  <si>
+    <t>tabraham</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>Jordan Zink</t>
+  </si>
+  <si>
+    <t>jzink</t>
+  </si>
+  <si>
+    <t>mclute</t>
+  </si>
+  <si>
+    <t>Maddy Clute</t>
+  </si>
+  <si>
+    <t>yuyangg</t>
+  </si>
+  <si>
+    <t>Yuyang Guo</t>
+  </si>
+  <si>
+    <t>Head Tutor</t>
+  </si>
+  <si>
+    <t>aayusha</t>
+  </si>
+  <si>
+    <t>advayak</t>
+  </si>
+  <si>
+    <t>afrank</t>
+  </si>
+  <si>
+    <t>anwu</t>
+  </si>
+  <si>
+    <t>dlbucci</t>
+  </si>
+  <si>
+    <t>eob</t>
+  </si>
+  <si>
+    <t>esmyers</t>
+  </si>
+  <si>
+    <t>gya</t>
+  </si>
+  <si>
+    <t>jacklinw</t>
+  </si>
+  <si>
+    <t>jrollins</t>
+  </si>
+  <si>
+    <t>mgazzola</t>
+  </si>
+  <si>
+    <t>mmatty</t>
+  </si>
+  <si>
+    <t>okahn</t>
+  </si>
+  <si>
+    <t>rokhinip</t>
+  </si>
+  <si>
+    <t>varunm</t>
+  </si>
+  <si>
+    <t>Aayush Agarwal</t>
+  </si>
+  <si>
+    <t>Advaya Krishna</t>
+  </si>
+  <si>
+    <t>Asa Frank</t>
+  </si>
+  <si>
+    <t>An Wu</t>
+  </si>
+  <si>
+    <t>Daniel Bucci</t>
+  </si>
+  <si>
+    <t>Elon Bauer</t>
+  </si>
+  <si>
+    <t>Ethan Myers</t>
+  </si>
+  <si>
+    <t>Jacklin Wu</t>
+  </si>
+  <si>
+    <t>Joseph Rollinson</t>
+  </si>
+  <si>
+    <t>Michael Matty</t>
+  </si>
+  <si>
+    <t>Owen Kahn</t>
+  </si>
+  <si>
+    <t>Rokhini Prabhu</t>
+  </si>
+  <si>
+    <t>Varun Murali</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>Z?</t>
+  </si>
+  <si>
+    <t>Gavi Adler</t>
+  </si>
+  <si>
+    <t>Mike Gazzola</t>
+  </si>
+  <si>
+    <t>noshlag</t>
+  </si>
+  <si>
+    <t>Nathan Oshlag</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>vebert</t>
+  </si>
+  <si>
+    <t>snalla</t>
+  </si>
+  <si>
+    <t>dbegos</t>
+  </si>
+  <si>
+    <t>yili1</t>
+  </si>
+  <si>
+    <t>cbrem</t>
+  </si>
+  <si>
+    <t>haozheg</t>
+  </si>
+  <si>
+    <t>dbora</t>
+  </si>
+  <si>
+    <t>lwzhang</t>
+  </si>
+  <si>
+    <t>jmfrye</t>
+  </si>
+  <si>
+    <t>treiter</t>
+  </si>
+  <si>
+    <t>kmao</t>
+  </si>
+  <si>
+    <t>dcushman</t>
+  </si>
+  <si>
+    <t>tcmoore</t>
+  </si>
+  <si>
+    <t>Shikha Nalla</t>
+  </si>
+  <si>
+    <t>DJ Begos</t>
+  </si>
+  <si>
+    <t>Connor Brem</t>
+  </si>
+  <si>
+    <t>Leon Zhang</t>
+  </si>
+  <si>
+    <t>Yi Li</t>
+  </si>
+  <si>
+    <t>Edison Gao</t>
+  </si>
+  <si>
+    <t>Disha Bora</t>
+  </si>
+  <si>
+    <t>Justin Frye</t>
+  </si>
+  <si>
+    <t>Tomer Reiter</t>
+  </si>
+  <si>
+    <t>Thomas Moore</t>
+  </si>
+  <si>
+    <t>Kechun Mao</t>
+  </si>
+  <si>
+    <t>Dan Cushman</t>
+  </si>
+  <si>
+    <t>Veronica Ebert</t>
+  </si>
+  <si>
+    <t>sguertin</t>
+  </si>
+  <si>
+    <t>shikunz</t>
+  </si>
+  <si>
+    <t>Shikun</t>
+  </si>
+  <si>
+    <t>mofarrel</t>
+  </si>
+  <si>
+    <t>acrigler</t>
+  </si>
+  <si>
+    <t>malehorn</t>
+  </si>
+  <si>
+    <t>akulk</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Stuart Guertin</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>Michael O'Farrell</t>
+  </si>
+  <si>
+    <t>Amelia Crigler</t>
+  </si>
+  <si>
+    <t>Brian Malehorn</t>
+  </si>
+  <si>
+    <t>Akul Kapoor</t>
+  </si>
+  <si>
+    <t>Instructor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -633,17 +903,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -667,12 +926,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1006,19 +1263,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T67"/>
+  <dimension ref="A1:T108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -1026,17 +1283,19 @@
     <col min="8" max="9" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1095,10 +1354,10 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1109,10 +1368,10 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1122,14 +1381,14 @@
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1137,10 +1396,10 @@
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -1148,10 +1407,10 @@
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1181,12 +1440,15 @@
       <c r="N6" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="S6" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -1194,10 +1456,10 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1205,220 +1467,232 @@
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15" customHeight="1">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>45</v>
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>49</v>
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>52</v>
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="S16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>60</v>
+      <c r="N17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" t="s">
+        <v>146</v>
+      </c>
+      <c r="R17" t="s">
+        <v>143</v>
+      </c>
+      <c r="S17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>62</v>
+    <row r="19" spans="1:19">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:19">
+      <c r="A21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>66</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1433,12 +1707,15 @@
       <c r="N21" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="4" t="s">
+      <c r="S21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1453,12 +1730,18 @@
       <c r="N22" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="4" t="s">
+      <c r="O22" t="s">
+        <v>43</v>
+      </c>
+      <c r="P22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1471,62 +1754,62 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>73</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>100</v>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>101</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>77</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>101</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>77</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>102</v>
       </c>
       <c r="M27" s="2" t="s">
@@ -1536,255 +1819,285 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>36</v>
+    <row r="28" spans="1:19">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>104</v>
+    <row r="29" spans="1:19">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>105</v>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>50</v>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>107</v>
+    <row r="32" spans="1:19">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>108</v>
+    <row r="33" spans="1:19">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>185</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>188</v>
+      <c r="N33" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P33" t="s">
+        <v>46</v>
+      </c>
+      <c r="R33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>185</v>
+      <c r="N34" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>109</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="N35" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>109</v>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>188</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>110</v>
+    <row r="37" spans="1:19">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="N37" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>189</v>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>111</v>
+      <c r="N38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O38" t="s">
+        <v>143</v>
+      </c>
+      <c r="S38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>79</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>79</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>38</v>
+        <v>155</v>
+      </c>
+      <c r="O40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
+        <v>189</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N41" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42" s="4" t="s">
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" t="s">
         <v>114</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
-      <c r="A43" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>115</v>
+    <row r="43" spans="1:19">
+      <c r="A43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>81</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="O43" t="s">
+        <v>43</v>
+      </c>
+      <c r="P43" t="s">
+        <v>143</v>
+      </c>
+      <c r="R43" t="s">
+        <v>142</v>
+      </c>
+      <c r="S43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
+        <v>115</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>81</v>
       </c>
       <c r="N44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O44" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:19">
+      <c r="A45" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" t="s">
         <v>117</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -1796,12 +2109,18 @@
       <c r="M45" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46" s="4" t="s">
+      <c r="O45" t="s">
+        <v>143</v>
+      </c>
+      <c r="P45" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" t="s">
         <v>119</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -1814,73 +2133,79 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
-      <c r="A47" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>121</v>
+    <row r="47" spans="1:19">
+      <c r="A47" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" t="s">
+        <v>123</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="A48" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>123</v>
+      <c r="O47" t="s">
+        <v>142</v>
+      </c>
+      <c r="P47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" t="s">
+        <v>121</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
-      <c r="A49" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>142</v>
+    <row r="49" spans="1:19">
+      <c r="A49" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" t="s">
+        <v>140</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
-      <c r="A50" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>140</v>
+    <row r="50" spans="1:19">
+      <c r="A50" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:19">
+      <c r="A51" t="s">
         <v>168</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" t="s">
         <v>141</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -1892,12 +2217,21 @@
       <c r="N51" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
-      <c r="A52" s="4" t="s">
+      <c r="O51" t="s">
+        <v>16</v>
+      </c>
+      <c r="P51" t="s">
+        <v>17</v>
+      </c>
+      <c r="S51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
+      <c r="A52" t="s">
         <v>169</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" t="s">
         <v>144</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -1910,11 +2244,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:19">
+      <c r="A53" t="s">
         <v>170</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" t="s">
         <v>145</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -1926,23 +2260,29 @@
       <c r="N53" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" s="4" t="s">
+      <c r="Q53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
+      <c r="A54" t="s">
         <v>171</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" t="s">
         <v>147</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="A55" s="4" t="s">
+      <c r="O54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
+      <c r="A55" t="s">
         <v>172</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" t="s">
         <v>148</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -1955,11 +2295,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:19">
+      <c r="A56" t="s">
         <v>173</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" t="s">
         <v>149</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -1971,12 +2311,15 @@
       <c r="N56" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" s="4" t="s">
+      <c r="O56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
+      <c r="A57" t="s">
         <v>186</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" t="s">
         <v>150</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -1989,11 +2332,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
-      <c r="A58" s="4" t="s">
+    <row r="58" spans="1:19">
+      <c r="A58" t="s">
         <v>174</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" t="s">
         <v>151</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -2006,11 +2349,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:19">
+      <c r="A59" t="s">
         <v>175</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" t="s">
         <v>152</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -2023,22 +2366,22 @@
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:19">
+      <c r="A60" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" t="s">
         <v>154</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:19">
+      <c r="A61" t="s">
         <v>177</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" t="s">
         <v>156</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -2051,11 +2394,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:19">
+      <c r="A62" t="s">
         <v>178</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" t="s">
         <v>157</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -2067,12 +2410,21 @@
       <c r="N62" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="63" spans="1:14">
-      <c r="A63" s="4" t="s">
+      <c r="O62" t="s">
+        <v>122</v>
+      </c>
+      <c r="P62" t="s">
+        <v>122</v>
+      </c>
+      <c r="S62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
+      <c r="A63" t="s">
         <v>179</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" t="s">
         <v>158</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -2084,12 +2436,15 @@
       <c r="N63" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="64" spans="1:14">
-      <c r="A64" s="4" t="s">
+      <c r="O63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
+      <c r="A64" t="s">
         <v>180</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" t="s">
         <v>159</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -2101,12 +2456,18 @@
       <c r="N64" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="A65" s="4" t="s">
+      <c r="R64" t="s">
+        <v>122</v>
+      </c>
+      <c r="S64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
+      <c r="A65" t="s">
         <v>181</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" t="s">
         <v>160</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2118,12 +2479,15 @@
       <c r="N65" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
-      <c r="A66" s="4" t="s">
+      <c r="O65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
+      <c r="A66" t="s">
         <v>184</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" t="s">
         <v>183</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -2135,12 +2499,15 @@
       <c r="N66" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:14">
-      <c r="A67" s="4" t="s">
+      <c r="O66" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19">
+      <c r="A67" t="s">
         <v>182</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" t="s">
         <v>161</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2153,7 +2520,782 @@
         <v>162</v>
       </c>
     </row>
+    <row r="68" spans="1:19">
+      <c r="A68" t="s">
+        <v>192</v>
+      </c>
+      <c r="B68" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O68" t="s">
+        <v>16</v>
+      </c>
+      <c r="P68" t="s">
+        <v>146</v>
+      </c>
+      <c r="S68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
+      <c r="A69" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" t="s">
+        <v>194</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O69" t="s">
+        <v>146</v>
+      </c>
+      <c r="P69" t="s">
+        <v>43</v>
+      </c>
+      <c r="R69" t="s">
+        <v>47</v>
+      </c>
+      <c r="S69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
+      <c r="A70" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P70" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>34</v>
+      </c>
+      <c r="R70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
+      <c r="A71" t="s">
+        <v>232</v>
+      </c>
+      <c r="B71" t="s">
+        <v>219</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P71" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>34</v>
+      </c>
+      <c r="R71" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19">
+      <c r="A72" t="s">
+        <v>225</v>
+      </c>
+      <c r="B72" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P72" t="s">
+        <v>17</v>
+      </c>
+      <c r="R72" t="s">
+        <v>118</v>
+      </c>
+      <c r="S72" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19">
+      <c r="A73" t="s">
+        <v>230</v>
+      </c>
+      <c r="B73" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P73" t="s">
+        <v>17</v>
+      </c>
+      <c r="R73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19">
+      <c r="A74" t="s">
+        <v>223</v>
+      </c>
+      <c r="B74" t="s">
+        <v>208</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P74" t="s">
+        <v>17</v>
+      </c>
+      <c r="R74" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19">
+      <c r="A75" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" t="s">
+        <v>216</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P75" t="s">
+        <v>17</v>
+      </c>
+      <c r="R75" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19">
+      <c r="A76" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" t="s">
+        <v>206</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P76" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19">
+      <c r="A77" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" t="s">
+        <v>209</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P77" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
+      <c r="A78" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P78" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19">
+      <c r="A79" t="s">
+        <v>227</v>
+      </c>
+      <c r="B79" t="s">
+        <v>212</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P79" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19">
+      <c r="A80" t="s">
+        <v>236</v>
+      </c>
+      <c r="B80" t="s">
+        <v>213</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P80" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
+      <c r="A81" t="s">
+        <v>228</v>
+      </c>
+      <c r="B81" t="s">
+        <v>214</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P81" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
+      <c r="A82" t="s">
+        <v>229</v>
+      </c>
+      <c r="B82" t="s">
+        <v>215</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="P82" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
+      <c r="A83" t="s">
+        <v>231</v>
+      </c>
+      <c r="B83" t="s">
+        <v>218</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P83" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19">
+      <c r="A84" t="s">
+        <v>233</v>
+      </c>
+      <c r="B84" t="s">
+        <v>220</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P84" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
+      <c r="A85" t="s">
+        <v>199</v>
+      </c>
+      <c r="B85" t="s">
+        <v>200</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P85" t="s">
+        <v>118</v>
+      </c>
+      <c r="R85" t="s">
+        <v>43</v>
+      </c>
+      <c r="S85" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
+      <c r="A86" t="s">
+        <v>202</v>
+      </c>
+      <c r="B86" t="s">
+        <v>201</v>
+      </c>
+      <c r="P86" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19">
+      <c r="A87" t="s">
+        <v>204</v>
+      </c>
+      <c r="B87" t="s">
+        <v>203</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P87" t="s">
+        <v>16</v>
+      </c>
+      <c r="R87" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19">
+      <c r="A88" t="s">
+        <v>196</v>
+      </c>
+      <c r="B88" t="s">
+        <v>197</v>
+      </c>
+      <c r="P88" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19">
+      <c r="A89" t="s">
+        <v>239</v>
+      </c>
+      <c r="B89" t="s">
+        <v>238</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>34</v>
+      </c>
+      <c r="R89" t="s">
+        <v>118</v>
+      </c>
+      <c r="S89" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
+      <c r="A90" t="s">
+        <v>266</v>
+      </c>
+      <c r="B90" t="s">
+        <v>241</v>
+      </c>
+      <c r="R90" t="s">
+        <v>118</v>
+      </c>
+      <c r="S90" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
+      <c r="A91" t="s">
+        <v>254</v>
+      </c>
+      <c r="B91" t="s">
+        <v>242</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R91" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
+      <c r="A92" t="s">
+        <v>255</v>
+      </c>
+      <c r="B92" t="s">
+        <v>243</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R92" t="s">
+        <v>142</v>
+      </c>
+      <c r="S92" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
+      <c r="A93" t="s">
+        <v>258</v>
+      </c>
+      <c r="B93" t="s">
+        <v>244</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="R93" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19">
+      <c r="A94" t="s">
+        <v>256</v>
+      </c>
+      <c r="B94" t="s">
+        <v>245</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R94" t="s">
+        <v>146</v>
+      </c>
+      <c r="S94" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19">
+      <c r="A95" t="s">
+        <v>259</v>
+      </c>
+      <c r="B95" t="s">
+        <v>246</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="R95" t="s">
+        <v>146</v>
+      </c>
+      <c r="S95" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19">
+      <c r="A96" t="s">
+        <v>260</v>
+      </c>
+      <c r="B96" t="s">
+        <v>247</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R96" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19">
+      <c r="A97" t="s">
+        <v>257</v>
+      </c>
+      <c r="B97" t="s">
+        <v>248</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R97" t="s">
+        <v>43</v>
+      </c>
+      <c r="S97" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19">
+      <c r="A98" t="s">
+        <v>261</v>
+      </c>
+      <c r="B98" t="s">
+        <v>249</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R98" t="s">
+        <v>43</v>
+      </c>
+      <c r="S98" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19">
+      <c r="A99" t="s">
+        <v>263</v>
+      </c>
+      <c r="B99" t="s">
+        <v>253</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R99" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19">
+      <c r="A100" t="s">
+        <v>262</v>
+      </c>
+      <c r="B100" t="s">
+        <v>250</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R100" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19">
+      <c r="A101" t="s">
+        <v>265</v>
+      </c>
+      <c r="B101" t="s">
+        <v>252</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R101" t="s">
+        <v>47</v>
+      </c>
+      <c r="S101" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19">
+      <c r="A102" t="s">
+        <v>264</v>
+      </c>
+      <c r="B102" t="s">
+        <v>251</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="R102" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19">
+      <c r="A103" t="s">
+        <v>275</v>
+      </c>
+      <c r="B103" t="s">
+        <v>267</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S103" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19">
+      <c r="A104" t="s">
+        <v>269</v>
+      </c>
+      <c r="B104" t="s">
+        <v>268</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="S104" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19">
+      <c r="A105" t="s">
+        <v>277</v>
+      </c>
+      <c r="B105" t="s">
+        <v>270</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="S105" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19">
+      <c r="A106" t="s">
+        <v>278</v>
+      </c>
+      <c r="B106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S106" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19">
+      <c r="A107" t="s">
+        <v>279</v>
+      </c>
+      <c r="B107" t="s">
+        <v>272</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="S107" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19">
+      <c r="A108" t="s">
+        <v>280</v>
+      </c>
+      <c r="B108" t="s">
+        <v>273</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="S108" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:T108">
+    <sortCondition ref="E2:E108"/>
+    <sortCondition ref="F2:F108"/>
+    <sortCondition ref="G2:G108"/>
+    <sortCondition ref="H2:H108"/>
+    <sortCondition ref="I2:I108"/>
+    <sortCondition ref="J2:J108"/>
+    <sortCondition ref="K2:K108"/>
+    <sortCondition ref="L2:L108"/>
+    <sortCondition ref="M2:M108"/>
+    <sortCondition ref="N2:N108"/>
+    <sortCondition ref="O2:O108"/>
+    <sortCondition ref="P2:P108"/>
+    <sortCondition ref="Q2:Q108"/>
+    <sortCondition ref="R2:R108"/>
+    <sortCondition ref="S2:S108"/>
+    <sortCondition ref="A2:A108"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>